<commit_message>
DOSINZAGE2-571-617: Added AccessionNumber and StudyInstanceUID to dataset and FHIR profile
</commit_message>
<xml_diff>
--- a/dataset/Dataset_MedMij_Beeldbeschikbaarheid_1.0.0-beta.1.xlsx
+++ b/dataset/Dataset_MedMij_Beeldbeschikbaarheid_1.0.0-beta.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luudslagter/Documents/git/MedMij-R4-ImageAvailability/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EA567B7-51D6-0D42-9007-78F6F69B0FB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9558F415-D0FC-9B44-B7A3-DF17225F53D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38560" yWindow="660" windowWidth="38080" windowHeight="19180" activeTab="1" xr2:uid="{B1E2DBBA-4EE0-4C1E-8D8A-42B6775C8263}"/>
+    <workbookView xWindow="29540" yWindow="660" windowWidth="34160" windowHeight="27980" activeTab="1" xr2:uid="{B1E2DBBA-4EE0-4C1E-8D8A-42B6775C8263}"/>
   </bookViews>
   <sheets>
     <sheet name="Beeld en verslag tijdlijn raadp" sheetId="3" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="244">
   <si>
     <t>Naam</t>
   </si>
@@ -759,6 +759,24 @@
 Elke zorginstelling werkt met een lijst van verrichtingen, die afleiden naar NZa-zorgactiviteiten. Een landelijke Verrichtingenthesaurus (gekoppeld aan NZa-zorgactiviteiten en SNOMED) is ontwikkeld met DHD en - op de combinatie-verrichtingen na - gereed voor gebruik door zorginstellingen in hun EPD/PACS.
 Idealiter is er een landelijke tabel van verrichtingen. Zolang dit niet landelijk wordt gebruikt én voor de onderzoeken die van voor de ingebruikname zijn, worden onderzoeken omschreven aan de hand van modaliteit en anatomisch gebied.
 Gebruik bij voorkeur de DHD code. Wanneer de DHD code er niet is, vul dit veld dan met modaliteit en anatomisch gebied door gebruik te maken van de vrije tekst mogelijkheid.</t>
+  </si>
+  <si>
+    <t>bbs-medmij-dataelement-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lokaal uniek ID (in het RIS) die is toegekend aan de aanvraag van het onderzoek. </t>
+  </si>
+  <si>
+    <t>bbs-medmij-dataelement-4</t>
+  </si>
+  <si>
+    <t>2.4. AccessionNumber</t>
+  </si>
+  <si>
+    <t>2.5. StudyInstanceUID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wereldwijd  uniek ID voor het onderzoek, toegekend door de modaliteit of het PACS.. </t>
   </si>
 </sst>
 </file>
@@ -1155,7 +1173,7 @@
     <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1203,12 +1221,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="25" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="25" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1273,6 +1285,15 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="25" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="25" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1682,60 +1703,55 @@
       </c>
     </row>
     <row r="2" spans="1:12" s="2" customFormat="1" ht="2" customHeight="1">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="31" t="s">
+      <c r="C2" s="53" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="31" t="s">
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="31" t="s">
+      <c r="K2" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="35" t="s">
+      <c r="L2" s="55" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:12" s="2" customFormat="1">
-      <c r="A3" s="32"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="36"/>
+      <c r="A3" s="54"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="G2:G3"/>
@@ -1743,6 +1759,11 @@
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="J2:J3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L2" r:id="rId1" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.0.1.7&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{3CDAD70A-3BBE-4CDA-810F-FA2B5C6B897A}"/>
@@ -1754,87 +1775,87 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B30DEB3F-E859-4BC8-9057-6D7475D627C0}">
-  <dimension ref="A1:O51"/>
+  <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="26.5" style="57" customWidth="1"/>
-    <col min="2" max="2" width="21.83203125" style="58" customWidth="1"/>
-    <col min="3" max="5" width="11" style="58" customWidth="1"/>
-    <col min="6" max="6" width="105.6640625" style="58" customWidth="1"/>
-    <col min="7" max="7" width="44" style="58" bestFit="1" customWidth="1"/>
-    <col min="8" max="241" width="11" style="58" customWidth="1"/>
-    <col min="242" max="16384" width="8.83203125" style="58"/>
+    <col min="1" max="1" width="26.5" style="51" customWidth="1"/>
+    <col min="2" max="2" width="21.83203125" style="52" customWidth="1"/>
+    <col min="3" max="5" width="11" style="52" customWidth="1"/>
+    <col min="6" max="6" width="105.6640625" style="52" customWidth="1"/>
+    <col min="7" max="7" width="44" style="52" bestFit="1" customWidth="1"/>
+    <col min="8" max="241" width="11" style="52" customWidth="1"/>
+    <col min="242" max="16384" width="8.83203125" style="52"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="10" customFormat="1">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="39" t="s">
+      <c r="G1" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="39" t="s">
+      <c r="I1" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="39" t="s">
+      <c r="J1" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="39" t="s">
+      <c r="K1" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="39" t="s">
+      <c r="L1" s="33" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="43" customFormat="1">
-      <c r="A2" s="40" t="s">
+    <row r="2" spans="1:15" s="37" customFormat="1">
+      <c r="A2" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="41" t="s">
+      <c r="C2" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="42"/>
-      <c r="F2" s="41" t="s">
+      <c r="E2" s="36"/>
+      <c r="F2" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="41" t="s">
+      <c r="J2" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="42" t="s">
+      <c r="L2" s="36" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="10" customFormat="1">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="38" t="s">
         <v>27</v>
       </c>
       <c r="B3" s="11" t="s">
@@ -1861,133 +1882,133 @@
       </c>
     </row>
     <row r="4" spans="1:15" s="10" customFormat="1">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="41" t="s">
+      <c r="C4" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="42" t="s">
+      <c r="E4" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="41" t="s">
+      <c r="F4" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="41" t="s">
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="41" t="s">
+      <c r="K4" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="L4" s="42" t="s">
+      <c r="L4" s="36" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:15" s="10" customFormat="1">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="41" t="s">
+      <c r="C5" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="42"/>
-      <c r="F5" s="41" t="s">
+      <c r="E5" s="36"/>
+      <c r="F5" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="41" t="s">
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="K5" s="41" t="s">
+      <c r="K5" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="L5" s="42" t="s">
+      <c r="L5" s="36" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:15" s="10" customFormat="1">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="41" t="s">
+      <c r="C6" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="42" t="s">
+      <c r="E6" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="41" t="s">
+      <c r="F6" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="41" t="s">
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="K6" s="41" t="s">
+      <c r="K6" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="L6" s="42" t="s">
+      <c r="L6" s="36" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:15" s="10" customFormat="1">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="41" t="s">
+      <c r="C7" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="42" t="s">
+      <c r="E7" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="41" t="s">
+      <c r="F7" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="41" t="s">
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="K7" s="41" t="s">
+      <c r="K7" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="L7" s="42" t="s">
+      <c r="L7" s="36" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:15" s="10" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A8" s="47" t="s">
+      <c r="A8" s="41" t="s">
         <v>51</v>
       </c>
       <c r="B8" s="11" t="s">
@@ -2019,284 +2040,284 @@
       </c>
     </row>
     <row r="9" spans="1:15" s="10" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A9" s="48" t="s">
+      <c r="A9" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="41" t="s">
+      <c r="C9" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="E9" s="42" t="s">
+      <c r="E9" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="F9" s="41" t="s">
+      <c r="F9" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="41" t="s">
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="K9" s="41" t="s">
+      <c r="K9" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="L9" s="42" t="s">
+      <c r="L9" s="36" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:15" s="10" customFormat="1">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="C10" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="41" t="s">
+      <c r="C10" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="42" t="s">
+      <c r="E10" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="F10" s="41" t="s">
+      <c r="F10" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="42" t="s">
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="J10" s="41" t="s">
+      <c r="J10" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="K10" s="41" t="s">
+      <c r="K10" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="L10" s="42" t="s">
+      <c r="L10" s="36" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:15" s="10" customFormat="1">
-      <c r="A11" s="49" t="s">
+      <c r="A11" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="C11" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="41" t="s">
+      <c r="C11" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="E11" s="42"/>
-      <c r="F11" s="41" t="s">
+      <c r="E11" s="36"/>
+      <c r="F11" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="41" t="s">
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="43"/>
-      <c r="L11" s="42"/>
+      <c r="K11" s="37"/>
+      <c r="L11" s="36"/>
     </row>
     <row r="12" spans="1:15" s="10" customFormat="1">
-      <c r="A12" s="50" t="s">
+      <c r="A12" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="B12" s="41" t="s">
+      <c r="B12" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="41" t="s">
+      <c r="C12" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="42"/>
-      <c r="F12" s="41" t="s">
+      <c r="E12" s="36"/>
+      <c r="F12" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="G12" s="43"/>
-      <c r="H12" s="42" t="s">
+      <c r="G12" s="37"/>
+      <c r="H12" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="I12" s="43"/>
-      <c r="J12" s="41" t="s">
+      <c r="I12" s="37"/>
+      <c r="J12" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="K12" s="41" t="s">
+      <c r="K12" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="L12" s="42"/>
+      <c r="L12" s="36"/>
     </row>
     <row r="13" spans="1:15" s="10" customFormat="1">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="41" t="s">
+      <c r="B13" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="C13" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="41" t="s">
+      <c r="C13" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="42" t="s">
+      <c r="E13" s="36" t="s">
         <v>56</v>
       </c>
       <c r="F13" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="41" t="s">
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="K13" s="41" t="s">
+      <c r="K13" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="L13" s="42"/>
+      <c r="L13" s="36"/>
     </row>
     <row r="14" spans="1:15" s="10" customFormat="1">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="B14" s="41" t="s">
+      <c r="B14" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="C14" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="41" t="s">
+      <c r="C14" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="42" t="s">
+      <c r="E14" s="36" t="s">
         <v>56</v>
       </c>
       <c r="F14" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="41" t="s">
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="K14" s="41" t="s">
+      <c r="K14" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="L14" s="42" t="s">
+      <c r="L14" s="36" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:15" s="10" customFormat="1" ht="105">
-      <c r="A15" s="45" t="s">
+      <c r="A15" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="B15" s="41" t="s">
+      <c r="B15" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="C15" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="41" t="s">
+      <c r="C15" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="42" t="s">
+      <c r="E15" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="F15" s="37" t="s">
+      <c r="F15" s="31" t="s">
         <v>237</v>
       </c>
-      <c r="G15" s="43"/>
-      <c r="H15" s="43"/>
-      <c r="I15" s="42" t="s">
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="36" t="s">
         <v>84</v>
       </c>
-      <c r="J15" s="41" t="s">
+      <c r="J15" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="K15" s="41" t="s">
+      <c r="K15" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="L15" s="42"/>
-      <c r="M15" s="51"/>
-      <c r="N15" s="51"/>
-      <c r="O15" s="51"/>
+      <c r="L15" s="36"/>
+      <c r="M15" s="45"/>
+      <c r="N15" s="45"/>
+      <c r="O15" s="45"/>
     </row>
     <row r="16" spans="1:15" s="10" customFormat="1" ht="16" customHeight="1">
-      <c r="A16" s="46" t="s">
+      <c r="A16" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="C16" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="41" t="s">
+      <c r="C16" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="42"/>
-      <c r="F16" s="51"/>
-      <c r="G16" s="43"/>
-      <c r="H16" s="42" t="s">
+      <c r="E16" s="36"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="I16" s="43"/>
-      <c r="J16" s="41" t="s">
+      <c r="I16" s="37"/>
+      <c r="J16" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="K16" s="41" t="s">
+      <c r="K16" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="L16" s="42"/>
-    </row>
-    <row r="17" spans="1:12" s="43" customFormat="1">
-      <c r="A17" s="52" t="s">
+      <c r="L16" s="36"/>
+    </row>
+    <row r="17" spans="1:12" s="37" customFormat="1">
+      <c r="A17" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="B17" s="41" t="s">
+      <c r="B17" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="C17" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="41" t="s">
+      <c r="C17" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="42" t="s">
+      <c r="E17" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="F17" s="53" t="s">
+      <c r="F17" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="H17" s="42" t="s">
+      <c r="H17" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="I17" s="42" t="s">
+      <c r="I17" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="J17" s="41" t="s">
+      <c r="J17" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="K17" s="41" t="s">
+      <c r="K17" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="L17" s="42"/>
+      <c r="L17" s="36"/>
     </row>
     <row r="18" spans="1:12" s="10" customFormat="1">
       <c r="A18" s="15" t="s">
@@ -2319,157 +2340,157 @@
       <c r="A19" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="B19" s="41" t="s">
+      <c r="B19" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="C19" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="41" t="s">
+      <c r="C19" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="42"/>
-      <c r="F19" s="41" t="s">
+      <c r="E19" s="36"/>
+      <c r="F19" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="G19" s="43"/>
-      <c r="H19" s="42" t="s">
+      <c r="G19" s="37"/>
+      <c r="H19" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="I19" s="43"/>
-      <c r="J19" s="41" t="s">
+      <c r="I19" s="37"/>
+      <c r="J19" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="K19" s="41" t="s">
+      <c r="K19" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="L19" s="42"/>
+      <c r="L19" s="36"/>
     </row>
     <row r="20" spans="1:12" s="10" customFormat="1">
-      <c r="A20" s="54" t="s">
+      <c r="A20" s="48" t="s">
         <v>101</v>
       </c>
-      <c r="B20" s="41" t="s">
+      <c r="B20" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="C20" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="41" t="s">
+      <c r="C20" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="42"/>
-      <c r="F20" s="41" t="s">
+      <c r="E20" s="36"/>
+      <c r="F20" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="G20" s="43"/>
-      <c r="H20" s="42" t="s">
+      <c r="G20" s="37"/>
+      <c r="H20" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="I20" s="43"/>
-      <c r="J20" s="41" t="s">
+      <c r="I20" s="37"/>
+      <c r="J20" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="K20" s="41" t="s">
+      <c r="K20" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="L20" s="42"/>
+      <c r="L20" s="36"/>
     </row>
     <row r="21" spans="1:12" s="10" customFormat="1" ht="15" customHeight="1">
-      <c r="A21" s="45" t="s">
+      <c r="A21" s="39" t="s">
         <v>105</v>
       </c>
-      <c r="B21" s="41" t="s">
+      <c r="B21" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="C21" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" s="41" t="s">
+      <c r="C21" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="E21" s="42" t="s">
+      <c r="E21" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="41" t="s">
+      <c r="F21" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="G21" s="41" t="s">
+      <c r="G21" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="H21" s="43"/>
-      <c r="I21" s="43"/>
-      <c r="J21" s="41" t="s">
+      <c r="H21" s="37"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="K21" s="41" t="s">
+      <c r="K21" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="L21" s="42"/>
+      <c r="L21" s="36"/>
     </row>
     <row r="22" spans="1:12" s="10" customFormat="1" ht="18" customHeight="1">
-      <c r="A22" s="45" t="s">
+      <c r="A22" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="B22" s="41" t="s">
+      <c r="B22" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="C22" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" s="41" t="s">
+      <c r="C22" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="42" t="s">
+      <c r="E22" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="F22" s="41" t="s">
+      <c r="F22" s="35" t="s">
         <v>112</v>
       </c>
-      <c r="G22" s="43"/>
-      <c r="H22" s="43"/>
-      <c r="I22" s="43"/>
-      <c r="J22" s="41" t="s">
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="K22" s="41" t="s">
+      <c r="K22" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="L22" s="42" t="s">
+      <c r="L22" s="36" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:12" s="10" customFormat="1">
-      <c r="A23" s="45" t="s">
+      <c r="A23" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="B23" s="41" t="s">
+      <c r="B23" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="C23" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" s="41" t="s">
+      <c r="C23" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="E23" s="42" t="s">
+      <c r="E23" s="36" t="s">
         <v>61</v>
       </c>
       <c r="F23" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="G23" s="43"/>
-      <c r="H23" s="43"/>
-      <c r="I23" s="42" t="s">
+      <c r="G23" s="37"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="36" t="s">
         <v>117</v>
       </c>
-      <c r="J23" s="41" t="s">
+      <c r="J23" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="K23" s="41" t="s">
+      <c r="K23" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="L23" s="42"/>
+      <c r="L23" s="36"/>
     </row>
     <row r="24" spans="1:12" s="10" customFormat="1">
       <c r="A24" s="15" t="s">
@@ -2504,309 +2525,309 @@
       </c>
     </row>
     <row r="25" spans="1:12" s="10" customFormat="1">
-      <c r="A25" s="46" t="s">
+      <c r="A25" s="40" t="s">
         <v>123</v>
       </c>
-      <c r="B25" s="41" t="s">
+      <c r="B25" s="35" t="s">
         <v>124</v>
       </c>
-      <c r="C25" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25" s="41" t="s">
+      <c r="C25" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="E25" s="42"/>
+      <c r="E25" s="36"/>
       <c r="F25" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="G25" s="43"/>
-      <c r="H25" s="43"/>
-      <c r="I25" s="43"/>
-      <c r="J25" s="41" t="s">
+      <c r="G25" s="37"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="K25" s="41" t="s">
+      <c r="K25" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="L25" s="42"/>
+      <c r="L25" s="36"/>
     </row>
     <row r="26" spans="1:12" s="10" customFormat="1">
       <c r="A26" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="B26" s="41" t="s">
+      <c r="B26" s="35" t="s">
         <v>127</v>
       </c>
-      <c r="C26" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D26" s="41" t="s">
+      <c r="C26" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="E26" s="42"/>
+      <c r="E26" s="36"/>
       <c r="F26" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="G26" s="43"/>
-      <c r="H26" s="42" t="s">
+      <c r="G26" s="37"/>
+      <c r="H26" s="36" t="s">
         <v>129</v>
       </c>
-      <c r="I26" s="43"/>
-      <c r="J26" s="41" t="s">
+      <c r="I26" s="37"/>
+      <c r="J26" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="K26" s="41" t="s">
+      <c r="K26" s="35" t="s">
         <v>130</v>
       </c>
-      <c r="L26" s="42"/>
+      <c r="L26" s="36"/>
     </row>
     <row r="27" spans="1:12" s="10" customFormat="1">
-      <c r="A27" s="45" t="s">
+      <c r="A27" s="39" t="s">
         <v>131</v>
       </c>
-      <c r="B27" s="41" t="s">
+      <c r="B27" s="35" t="s">
         <v>132</v>
       </c>
-      <c r="C27" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D27" s="41" t="s">
+      <c r="C27" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="E27" s="42" t="s">
+      <c r="E27" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="F27" s="41" t="s">
+      <c r="F27" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="G27" s="41" t="s">
+      <c r="G27" s="35" t="s">
         <v>134</v>
       </c>
-      <c r="H27" s="43"/>
-      <c r="I27" s="43"/>
-      <c r="J27" s="41" t="s">
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="K27" s="41" t="s">
+      <c r="K27" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="L27" s="42"/>
+      <c r="L27" s="36"/>
     </row>
     <row r="28" spans="1:12" s="10" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A28" s="46" t="s">
+      <c r="A28" s="40" t="s">
         <v>136</v>
       </c>
-      <c r="B28" s="41" t="s">
+      <c r="B28" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="C28" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" s="41" t="s">
+      <c r="C28" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="E28" s="42"/>
-      <c r="F28" s="41" t="s">
+      <c r="E28" s="36"/>
+      <c r="F28" s="35" t="s">
         <v>138</v>
       </c>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="41" t="s">
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="K28" s="41" t="s">
+      <c r="K28" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="L28" s="42" t="s">
+      <c r="L28" s="36" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="29" spans="1:12" s="10" customFormat="1">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="39" t="s">
         <v>140</v>
       </c>
-      <c r="B29" s="41" t="s">
+      <c r="B29" s="35" t="s">
         <v>141</v>
       </c>
-      <c r="C29" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D29" s="41" t="s">
+      <c r="C29" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="E29" s="42" t="s">
+      <c r="E29" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="F29" s="41" t="s">
+      <c r="F29" s="35" t="s">
         <v>142</v>
       </c>
-      <c r="G29" s="43"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="43"/>
-      <c r="J29" s="41" t="s">
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="K29" s="41" t="s">
+      <c r="K29" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="L29" s="42" t="s">
+      <c r="L29" s="36" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="30" spans="1:12" s="10" customFormat="1">
-      <c r="A30" s="46" t="s">
+      <c r="A30" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="B30" s="41" t="s">
+      <c r="B30" s="35" t="s">
         <v>145</v>
       </c>
-      <c r="C30" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D30" s="41" t="s">
+      <c r="C30" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="E30" s="42"/>
-      <c r="F30" s="41" t="s">
+      <c r="E30" s="36"/>
+      <c r="F30" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="G30" s="43"/>
-      <c r="H30" s="43"/>
-      <c r="I30" s="43"/>
-      <c r="J30" s="41" t="s">
+      <c r="G30" s="37"/>
+      <c r="H30" s="37"/>
+      <c r="I30" s="37"/>
+      <c r="J30" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="K30" s="41" t="s">
+      <c r="K30" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="L30" s="42" t="s">
+      <c r="L30" s="36" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="31" spans="1:12" s="10" customFormat="1">
-      <c r="A31" s="45" t="s">
+      <c r="A31" s="39" t="s">
         <v>147</v>
       </c>
-      <c r="B31" s="41" t="s">
+      <c r="B31" s="35" t="s">
         <v>148</v>
       </c>
-      <c r="C31" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D31" s="41" t="s">
+      <c r="C31" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="E31" s="42" t="s">
+      <c r="E31" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="F31" s="41" t="s">
+      <c r="F31" s="35" t="s">
         <v>149</v>
       </c>
-      <c r="G31" s="43"/>
-      <c r="H31" s="43"/>
-      <c r="I31" s="43"/>
-      <c r="J31" s="41" t="s">
+      <c r="G31" s="37"/>
+      <c r="H31" s="37"/>
+      <c r="I31" s="37"/>
+      <c r="J31" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="K31" s="41" t="s">
+      <c r="K31" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="L31" s="42" t="s">
+      <c r="L31" s="36" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="32" spans="1:12" s="10" customFormat="1">
-      <c r="A32" s="45" t="s">
+      <c r="A32" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="B32" s="41" t="s">
+      <c r="B32" s="35" t="s">
         <v>152</v>
       </c>
-      <c r="C32" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D32" s="41" t="s">
+      <c r="C32" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="E32" s="42" t="s">
+      <c r="E32" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="F32" s="41" t="s">
+      <c r="F32" s="35" t="s">
         <v>153</v>
       </c>
-      <c r="G32" s="43"/>
-      <c r="H32" s="43"/>
-      <c r="I32" s="43"/>
-      <c r="J32" s="41" t="s">
+      <c r="G32" s="37"/>
+      <c r="H32" s="37"/>
+      <c r="I32" s="37"/>
+      <c r="J32" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="K32" s="41" t="s">
+      <c r="K32" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="L32" s="42" t="s">
+      <c r="L32" s="36" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="33" spans="1:12" s="10" customFormat="1">
-      <c r="A33" s="45" t="s">
+      <c r="A33" s="39" t="s">
         <v>155</v>
       </c>
-      <c r="B33" s="41" t="s">
+      <c r="B33" s="35" t="s">
         <v>156</v>
       </c>
-      <c r="C33" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D33" s="41" t="s">
+      <c r="C33" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="E33" s="42" t="s">
+      <c r="E33" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="F33" s="41" t="s">
+      <c r="F33" s="35" t="s">
         <v>157</v>
       </c>
-      <c r="G33" s="43"/>
-      <c r="H33" s="42" t="s">
+      <c r="G33" s="37"/>
+      <c r="H33" s="36" t="s">
         <v>158</v>
       </c>
-      <c r="I33" s="42" t="s">
+      <c r="I33" s="36" t="s">
         <v>159</v>
       </c>
-      <c r="J33" s="41" t="s">
+      <c r="J33" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="K33" s="41" t="s">
+      <c r="K33" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="L33" s="42"/>
-    </row>
-    <row r="34" spans="1:12" s="43" customFormat="1">
-      <c r="A34" s="46" t="s">
+      <c r="L33" s="36"/>
+    </row>
+    <row r="34" spans="1:12" s="37" customFormat="1">
+      <c r="A34" s="40" t="s">
         <v>160</v>
       </c>
-      <c r="B34" s="41" t="s">
+      <c r="B34" s="35" t="s">
         <v>161</v>
       </c>
-      <c r="C34" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D34" s="41" t="s">
+      <c r="C34" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="E34" s="42"/>
-      <c r="F34" s="41" t="s">
+      <c r="E34" s="36"/>
+      <c r="F34" s="35" t="s">
         <v>162</v>
       </c>
-      <c r="J34" s="41" t="s">
+      <c r="J34" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="K34" s="41" t="s">
+      <c r="K34" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="L34" s="42"/>
+      <c r="L34" s="36"/>
     </row>
     <row r="35" spans="1:12" s="10" customFormat="1">
       <c r="A35" s="11" t="s">
@@ -2837,348 +2858,348 @@
       <c r="L35" s="12"/>
     </row>
     <row r="36" spans="1:12" s="10" customFormat="1">
-      <c r="A36" s="45" t="s">
+      <c r="A36" s="39" t="s">
         <v>166</v>
       </c>
-      <c r="B36" s="41" t="s">
+      <c r="B36" s="35" t="s">
         <v>167</v>
       </c>
-      <c r="C36" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D36" s="41" t="s">
+      <c r="C36" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="E36" s="42" t="s">
+      <c r="E36" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="F36" s="41" t="s">
+      <c r="F36" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="G36" s="41" t="s">
+      <c r="G36" s="35" t="s">
         <v>134</v>
       </c>
-      <c r="H36" s="43"/>
-      <c r="I36" s="43"/>
-      <c r="J36" s="41" t="s">
+      <c r="H36" s="37"/>
+      <c r="I36" s="37"/>
+      <c r="J36" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="K36" s="41" t="s">
+      <c r="K36" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="L36" s="42"/>
+      <c r="L36" s="36"/>
     </row>
     <row r="37" spans="1:12" s="10" customFormat="1" ht="18" customHeight="1">
-      <c r="A37" s="46" t="s">
+      <c r="A37" s="40" t="s">
         <v>168</v>
       </c>
-      <c r="B37" s="41" t="s">
+      <c r="B37" s="35" t="s">
         <v>169</v>
       </c>
-      <c r="C37" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D37" s="41" t="s">
+      <c r="C37" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="E37" s="42"/>
-      <c r="F37" s="41" t="s">
+      <c r="E37" s="36"/>
+      <c r="F37" s="35" t="s">
         <v>138</v>
       </c>
-      <c r="G37" s="43"/>
-      <c r="H37" s="43"/>
-      <c r="I37" s="43"/>
-      <c r="J37" s="41" t="s">
+      <c r="G37" s="37"/>
+      <c r="H37" s="37"/>
+      <c r="I37" s="37"/>
+      <c r="J37" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="K37" s="41" t="s">
+      <c r="K37" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="L37" s="42" t="s">
+      <c r="L37" s="36" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="38" spans="1:12" s="10" customFormat="1">
-      <c r="A38" s="45" t="s">
+      <c r="A38" s="39" t="s">
         <v>170</v>
       </c>
-      <c r="B38" s="41" t="s">
+      <c r="B38" s="35" t="s">
         <v>171</v>
       </c>
-      <c r="C38" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D38" s="41" t="s">
+      <c r="C38" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="E38" s="42" t="s">
+      <c r="E38" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="F38" s="41" t="s">
+      <c r="F38" s="35" t="s">
         <v>142</v>
       </c>
-      <c r="G38" s="43"/>
-      <c r="H38" s="43"/>
-      <c r="I38" s="43"/>
-      <c r="J38" s="41" t="s">
+      <c r="G38" s="37"/>
+      <c r="H38" s="37"/>
+      <c r="I38" s="37"/>
+      <c r="J38" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="K38" s="41" t="s">
+      <c r="K38" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="L38" s="42" t="s">
+      <c r="L38" s="36" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="39" spans="1:12" s="10" customFormat="1">
-      <c r="A39" s="46" t="s">
+      <c r="A39" s="40" t="s">
         <v>172</v>
       </c>
-      <c r="B39" s="41" t="s">
+      <c r="B39" s="35" t="s">
         <v>173</v>
       </c>
-      <c r="C39" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D39" s="41" t="s">
+      <c r="C39" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="E39" s="42"/>
-      <c r="F39" s="41" t="s">
+      <c r="E39" s="36"/>
+      <c r="F39" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="G39" s="43"/>
-      <c r="H39" s="43"/>
-      <c r="I39" s="43"/>
-      <c r="J39" s="41" t="s">
+      <c r="G39" s="37"/>
+      <c r="H39" s="37"/>
+      <c r="I39" s="37"/>
+      <c r="J39" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="K39" s="41" t="s">
+      <c r="K39" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="L39" s="42" t="s">
+      <c r="L39" s="36" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="40" spans="1:12" s="10" customFormat="1">
-      <c r="A40" s="45" t="s">
+      <c r="A40" s="39" t="s">
         <v>174</v>
       </c>
-      <c r="B40" s="41" t="s">
+      <c r="B40" s="35" t="s">
         <v>175</v>
       </c>
-      <c r="C40" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D40" s="41" t="s">
+      <c r="C40" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="E40" s="42" t="s">
+      <c r="E40" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="F40" s="41" t="s">
+      <c r="F40" s="35" t="s">
         <v>149</v>
       </c>
-      <c r="G40" s="43"/>
-      <c r="H40" s="43"/>
-      <c r="I40" s="43"/>
-      <c r="J40" s="41" t="s">
+      <c r="G40" s="37"/>
+      <c r="H40" s="37"/>
+      <c r="I40" s="37"/>
+      <c r="J40" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="K40" s="41" t="s">
+      <c r="K40" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="L40" s="42" t="s">
+      <c r="L40" s="36" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="41" spans="1:12" s="10" customFormat="1">
-      <c r="A41" s="45" t="s">
+      <c r="A41" s="39" t="s">
         <v>176</v>
       </c>
-      <c r="B41" s="41" t="s">
+      <c r="B41" s="35" t="s">
         <v>177</v>
       </c>
-      <c r="C41" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D41" s="41" t="s">
+      <c r="C41" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="E41" s="42" t="s">
+      <c r="E41" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="F41" s="41" t="s">
+      <c r="F41" s="35" t="s">
         <v>153</v>
       </c>
-      <c r="G41" s="43"/>
-      <c r="H41" s="43"/>
-      <c r="I41" s="43"/>
-      <c r="J41" s="41" t="s">
+      <c r="G41" s="37"/>
+      <c r="H41" s="37"/>
+      <c r="I41" s="37"/>
+      <c r="J41" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="K41" s="41" t="s">
+      <c r="K41" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="L41" s="42" t="s">
+      <c r="L41" s="36" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="42" spans="1:12" s="10" customFormat="1">
-      <c r="A42" s="45" t="s">
+      <c r="A42" s="39" t="s">
         <v>178</v>
       </c>
-      <c r="B42" s="41" t="s">
+      <c r="B42" s="35" t="s">
         <v>179</v>
       </c>
-      <c r="C42" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D42" s="41" t="s">
+      <c r="C42" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="E42" s="42" t="s">
+      <c r="E42" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="F42" s="41" t="s">
+      <c r="F42" s="35" t="s">
         <v>157</v>
       </c>
-      <c r="G42" s="43"/>
-      <c r="H42" s="42" t="s">
+      <c r="G42" s="37"/>
+      <c r="H42" s="36" t="s">
         <v>158</v>
       </c>
-      <c r="I42" s="42" t="s">
+      <c r="I42" s="36" t="s">
         <v>159</v>
       </c>
-      <c r="J42" s="41" t="s">
+      <c r="J42" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="K42" s="41" t="s">
+      <c r="K42" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="L42" s="42"/>
+      <c r="L42" s="36"/>
     </row>
     <row r="43" spans="1:12" s="10" customFormat="1">
-      <c r="A43" s="45" t="s">
+      <c r="A43" s="39" t="s">
         <v>180</v>
       </c>
-      <c r="B43" s="41" t="s">
+      <c r="B43" s="35" t="s">
         <v>181</v>
       </c>
-      <c r="C43" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D43" s="41" t="s">
+      <c r="C43" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D43" s="35" t="s">
         <v>182</v>
       </c>
-      <c r="E43" s="42" t="s">
+      <c r="E43" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="F43" s="41" t="s">
+      <c r="F43" s="35" t="s">
         <v>183</v>
       </c>
-      <c r="G43" s="43"/>
-      <c r="H43" s="43"/>
-      <c r="I43" s="42" t="s">
+      <c r="G43" s="37"/>
+      <c r="H43" s="37"/>
+      <c r="I43" s="36" t="s">
         <v>184</v>
       </c>
-      <c r="J43" s="41" t="s">
+      <c r="J43" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="K43" s="41" t="s">
+      <c r="K43" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="L43" s="42" t="s">
+      <c r="L43" s="36" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="44" spans="1:12" s="10" customFormat="1">
-      <c r="A44" s="55" t="s">
+      <c r="A44" s="49" t="s">
         <v>186</v>
       </c>
-      <c r="B44" s="41" t="s">
+      <c r="B44" s="35" t="s">
         <v>187</v>
       </c>
-      <c r="C44" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D44" s="56" t="s">
+      <c r="C44" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="E44" s="42"/>
-      <c r="F44" s="41" t="s">
+      <c r="E44" s="36"/>
+      <c r="F44" s="35" t="s">
         <v>188</v>
       </c>
-      <c r="G44" s="43"/>
-      <c r="H44" s="43"/>
-      <c r="I44" s="43"/>
-      <c r="J44" s="41" t="s">
+      <c r="G44" s="37"/>
+      <c r="H44" s="37"/>
+      <c r="I44" s="37"/>
+      <c r="J44" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="K44" s="41" t="s">
+      <c r="K44" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="L44" s="42"/>
+      <c r="L44" s="36"/>
     </row>
     <row r="45" spans="1:12" s="10" customFormat="1">
-      <c r="A45" s="45" t="s">
+      <c r="A45" s="39" t="s">
         <v>189</v>
       </c>
-      <c r="B45" s="41" t="s">
+      <c r="B45" s="35" t="s">
         <v>190</v>
       </c>
-      <c r="C45" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D45" s="41" t="s">
+      <c r="C45" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D45" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="E45" s="42" t="s">
+      <c r="E45" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="F45" s="41" t="s">
+      <c r="F45" s="35" t="s">
         <v>191</v>
       </c>
-      <c r="G45" s="43"/>
-      <c r="H45" s="43"/>
-      <c r="I45" s="43"/>
-      <c r="J45" s="41" t="s">
+      <c r="G45" s="37"/>
+      <c r="H45" s="37"/>
+      <c r="I45" s="37"/>
+      <c r="J45" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="K45" s="41" t="s">
+      <c r="K45" s="35" t="s">
         <v>192</v>
       </c>
-      <c r="L45" s="42"/>
+      <c r="L45" s="36"/>
     </row>
     <row r="46" spans="1:12" s="10" customFormat="1">
-      <c r="A46" s="45" t="s">
+      <c r="A46" s="39" t="s">
         <v>193</v>
       </c>
-      <c r="B46" s="41" t="s">
+      <c r="B46" s="35" t="s">
         <v>194</v>
       </c>
-      <c r="C46" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D46" s="41" t="s">
+      <c r="C46" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D46" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="E46" s="42" t="s">
+      <c r="E46" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="F46" s="41" t="s">
+      <c r="F46" s="35" t="s">
         <v>195</v>
       </c>
-      <c r="G46" s="43"/>
-      <c r="H46" s="43"/>
-      <c r="I46" s="43"/>
-      <c r="J46" s="41" t="s">
+      <c r="G46" s="37"/>
+      <c r="H46" s="37"/>
+      <c r="I46" s="37"/>
+      <c r="J46" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="K46" s="41" t="s">
+      <c r="K46" s="35" t="s">
         <v>192</v>
       </c>
-      <c r="L46" s="42"/>
+      <c r="L46" s="36"/>
     </row>
     <row r="47" spans="1:12" s="10" customFormat="1">
       <c r="A47" s="15" t="s">
@@ -3200,99 +3221,101 @@
         <v>200</v>
       </c>
       <c r="I47" s="12"/>
-      <c r="J47" s="11"/>
+      <c r="J47" s="11" t="s">
+        <v>19</v>
+      </c>
       <c r="K47" s="11" t="s">
         <v>192</v>
       </c>
       <c r="L47" s="12"/>
     </row>
     <row r="48" spans="1:12" s="10" customFormat="1">
-      <c r="A48" s="55" t="s">
+      <c r="A48" s="49" t="s">
         <v>201</v>
       </c>
-      <c r="B48" s="41" t="s">
+      <c r="B48" s="35" t="s">
         <v>202</v>
       </c>
-      <c r="C48" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D48" s="41" t="s">
+      <c r="C48" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D48" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="E48" s="42"/>
-      <c r="F48" s="41" t="s">
+      <c r="E48" s="36"/>
+      <c r="F48" s="35" t="s">
         <v>232</v>
       </c>
-      <c r="G48" s="43"/>
-      <c r="H48" s="43"/>
-      <c r="I48" s="43"/>
-      <c r="J48" s="41" t="s">
+      <c r="G48" s="37"/>
+      <c r="H48" s="37"/>
+      <c r="I48" s="37"/>
+      <c r="J48" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="K48" s="41" t="s">
+      <c r="K48" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="L48" s="42"/>
+      <c r="L48" s="36"/>
     </row>
     <row r="49" spans="1:12" s="10" customFormat="1">
-      <c r="A49" s="45" t="s">
+      <c r="A49" s="39" t="s">
         <v>203</v>
       </c>
-      <c r="B49" s="41" t="s">
+      <c r="B49" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="C49" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D49" s="41" t="s">
+      <c r="C49" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D49" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="E49" s="42" t="s">
+      <c r="E49" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="F49" s="41" t="s">
+      <c r="F49" s="35" t="s">
         <v>205</v>
       </c>
-      <c r="G49" s="43"/>
-      <c r="H49" s="43"/>
-      <c r="I49" s="43"/>
-      <c r="J49" s="41" t="s">
+      <c r="G49" s="37"/>
+      <c r="H49" s="37"/>
+      <c r="I49" s="37"/>
+      <c r="J49" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="K49" s="41" t="s">
+      <c r="K49" s="35" t="s">
         <v>206</v>
       </c>
-      <c r="L49" s="42"/>
+      <c r="L49" s="36"/>
     </row>
     <row r="50" spans="1:12" s="10" customFormat="1">
-      <c r="A50" s="45" t="s">
+      <c r="A50" s="39" t="s">
         <v>207</v>
       </c>
-      <c r="B50" s="41" t="s">
+      <c r="B50" s="35" t="s">
         <v>208</v>
       </c>
-      <c r="C50" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D50" s="41" t="s">
+      <c r="C50" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D50" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="E50" s="42" t="s">
+      <c r="E50" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="F50" s="41" t="s">
+      <c r="F50" s="35" t="s">
         <v>209</v>
       </c>
-      <c r="G50" s="43"/>
-      <c r="H50" s="43"/>
-      <c r="I50" s="43"/>
-      <c r="J50" s="41" t="s">
+      <c r="G50" s="37"/>
+      <c r="H50" s="37"/>
+      <c r="I50" s="37"/>
+      <c r="J50" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="K50" s="41" t="s">
+      <c r="K50" s="35" t="s">
         <v>206</v>
       </c>
-      <c r="L50" s="42"/>
+      <c r="L50" s="36"/>
     </row>
     <row r="51" spans="1:12" s="10" customFormat="1">
       <c r="A51" s="15" t="s">
@@ -3314,11 +3337,73 @@
         <v>212</v>
       </c>
       <c r="I51" s="12"/>
-      <c r="J51" s="11"/>
+      <c r="J51" s="11" t="s">
+        <v>19</v>
+      </c>
       <c r="K51" s="11" t="s">
         <v>206</v>
       </c>
       <c r="L51" s="12"/>
+    </row>
+    <row r="52" spans="1:12" s="10" customFormat="1">
+      <c r="A52" s="59" t="s">
+        <v>241</v>
+      </c>
+      <c r="B52" s="35" t="s">
+        <v>238</v>
+      </c>
+      <c r="C52" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D52" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="E52" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="F52" s="35" t="s">
+        <v>239</v>
+      </c>
+      <c r="G52" s="37"/>
+      <c r="H52" s="37"/>
+      <c r="I52" s="36"/>
+      <c r="J52" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="K52" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="L52" s="36"/>
+    </row>
+    <row r="53" spans="1:12" s="10" customFormat="1">
+      <c r="A53" s="59" t="s">
+        <v>242</v>
+      </c>
+      <c r="B53" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="C53" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D53" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="E53" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="F53" s="35" t="s">
+        <v>243</v>
+      </c>
+      <c r="G53" s="37"/>
+      <c r="H53" s="37"/>
+      <c r="I53" s="36"/>
+      <c r="J53" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="K53" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="L53" s="36"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:N51" xr:uid="{B30DEB3F-E859-4BC8-9057-6D7475D627C0}"/>
@@ -3437,6 +3522,8 @@
     <hyperlink ref="H17" r:id="rId111" display="http://decor.nictiz.nl/decor/services/RedirectTerminology?codeSystem=2.16.840.1.113883.6.96&amp;conceptId=363698007&amp;language=nl-NL&amp;prefix=bbs-&amp;version=2024-02-08T09:28:09" xr:uid="{58172FD2-70FC-4673-BF70-D6AE18467415}"/>
     <hyperlink ref="E17" r:id="rId112" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{3D0023D3-652A-4840-9808-3B2E5DA099D0}"/>
     <hyperlink ref="E18" r:id="rId113" location="/bbs-/terminology/valueset/2.16.840.1.113883.2.4.3.11.60.40.2.20.7.2/2020-09-01T00:00:00" xr:uid="{4B3833E8-D6ED-4EC3-8D1E-0F1FF55B206E}"/>
+    <hyperlink ref="E52" r:id="rId114" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{06898B6A-A0ED-0244-9A16-72B56DEBED42}"/>
+    <hyperlink ref="E53" r:id="rId115" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{EABED256-857D-2642-BE3E-5AD20C03336E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4264,26 +4351,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7be6589a-2b09-4451-a4d9-5c4f513f6c62" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100597771DCE5E0DD409E6796B5544574D3" ma:contentTypeVersion="14" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="1f155c61874143f60c84865cea76726f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7be6589a-2b09-4451-a4d9-5c4f513f6c62" xmlns:ns3="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7515b2bcca035c7557d524d6ba7a724c" ns2:_="" ns3:_="">
     <xsd:import namespace="7be6589a-2b09-4451-a4d9-5c4f513f6c62"/>
@@ -4512,26 +4579,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A9F8A2F-C3FF-4FEC-AF19-26E26DE76F65}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7"/>
-    <ds:schemaRef ds:uri="7be6589a-2b09-4451-a4d9-5c4f513f6c62"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD20EF80-7752-41E2-9F6E-5CDF83210C62}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7be6589a-2b09-4451-a4d9-5c4f513f6c62" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{815FF2A9-0500-4E41-8F16-110FB0128C02}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4550,6 +4618,25 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD20EF80-7752-41E2-9F6E-5CDF83210C62}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A9F8A2F-C3FF-4FEC-AF19-26E26DE76F65}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7"/>
+    <ds:schemaRef ds:uri="7be6589a-2b09-4451-a4d9-5c4f513f6c62"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{72c2d0db-a1e3-4b16-91a1-67936a5cf3bf}" enabled="0" method="" siteId="{72c2d0db-a1e3-4b16-91a1-67936a5cf3bf}" removed="1"/>

</xml_diff>

<commit_message>
DOSINZAGE2-571-617: Textual finetuning of dataset
</commit_message>
<xml_diff>
--- a/dataset/Dataset_MedMij_Beeldbeschikbaarheid_1.0.0-beta.1.xlsx
+++ b/dataset/Dataset_MedMij_Beeldbeschikbaarheid_1.0.0-beta.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luudslagter/Documents/git/MedMij-R4-ImageAvailability/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9558F415-D0FC-9B44-B7A3-DF17225F53D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74104CF2-C1C7-2D4D-B889-A22058A398B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29540" yWindow="660" windowWidth="34160" windowHeight="27980" activeTab="1" xr2:uid="{B1E2DBBA-4EE0-4C1E-8D8A-42B6775C8263}"/>
   </bookViews>
@@ -764,9 +764,6 @@
     <t>bbs-medmij-dataelement-3</t>
   </si>
   <si>
-    <t xml:space="preserve">Lokaal uniek ID (in het RIS) die is toegekend aan de aanvraag van het onderzoek. </t>
-  </si>
-  <si>
     <t>bbs-medmij-dataelement-4</t>
   </si>
   <si>
@@ -776,14 +773,17 @@
     <t>2.5. StudyInstanceUID</t>
   </si>
   <si>
-    <t xml:space="preserve">Wereldwijd  uniek ID voor het onderzoek, toegekend door de modaliteit of het PACS.. </t>
+    <t>Wereldwijd  uniek ID voor het onderzoek, toegekend door de modaliteit of het PACS.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lokaal uniek ID (in het RIS) die is toegekend aan het onderzoek. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -907,6 +907,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="12"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
@@ -1289,11 +1295,11 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="25" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="25" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1715,7 +1721,7 @@
       <c r="D2" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="55" t="s">
+      <c r="E2" s="57" t="s">
         <v>16</v>
       </c>
       <c r="F2" s="53" t="s">
@@ -1724,15 +1730,15 @@
       <c r="G2" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
       <c r="J2" s="53" t="s">
         <v>19</v>
       </c>
       <c r="K2" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="55" t="s">
+      <c r="L2" s="57" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1741,17 +1747,22 @@
       <c r="B3" s="54"/>
       <c r="C3" s="54"/>
       <c r="D3" s="54"/>
-      <c r="E3" s="56"/>
+      <c r="E3" s="58"/>
       <c r="F3" s="54"/>
       <c r="G3" s="54"/>
-      <c r="H3" s="58"/>
-      <c r="I3" s="58"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
       <c r="J3" s="54"/>
       <c r="K3" s="54"/>
-      <c r="L3" s="56"/>
+      <c r="L3" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="G2:G3"/>
@@ -1759,11 +1770,6 @@
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="J2:J3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L2" r:id="rId1" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.0.1.7&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{3CDAD70A-3BBE-4CDA-810F-FA2B5C6B897A}"/>
@@ -1778,7 +1784,7 @@
   <dimension ref="A1:O53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -3347,7 +3353,7 @@
     </row>
     <row r="52" spans="1:12" s="10" customFormat="1">
       <c r="A52" s="59" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B52" s="35" t="s">
         <v>238</v>
@@ -3362,7 +3368,7 @@
         <v>16</v>
       </c>
       <c r="F52" s="35" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="G52" s="37"/>
       <c r="H52" s="37"/>
@@ -3377,10 +3383,10 @@
     </row>
     <row r="53" spans="1:12" s="10" customFormat="1">
       <c r="A53" s="59" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B53" s="35" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C53" s="35" t="s">
         <v>14</v>
@@ -3392,7 +3398,7 @@
         <v>16</v>
       </c>
       <c r="F53" s="35" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G53" s="37"/>
       <c r="H53" s="37"/>
@@ -4351,6 +4357,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7be6589a-2b09-4451-a4d9-5c4f513f6c62" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100597771DCE5E0DD409E6796B5544574D3" ma:contentTypeVersion="14" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="1f155c61874143f60c84865cea76726f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7be6589a-2b09-4451-a4d9-5c4f513f6c62" xmlns:ns3="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7515b2bcca035c7557d524d6ba7a724c" ns2:_="" ns3:_="">
     <xsd:import namespace="7be6589a-2b09-4451-a4d9-5c4f513f6c62"/>
@@ -4579,27 +4605,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A9F8A2F-C3FF-4FEC-AF19-26E26DE76F65}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7"/>
+    <ds:schemaRef ds:uri="7be6589a-2b09-4451-a4d9-5c4f513f6c62"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7be6589a-2b09-4451-a4d9-5c4f513f6c62" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD20EF80-7752-41E2-9F6E-5CDF83210C62}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{815FF2A9-0500-4E41-8F16-110FB0128C02}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4618,25 +4643,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD20EF80-7752-41E2-9F6E-5CDF83210C62}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A9F8A2F-C3FF-4FEC-AF19-26E26DE76F65}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7"/>
-    <ds:schemaRef ds:uri="7be6589a-2b09-4451-a4d9-5c4f513f6c62"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{72c2d0db-a1e3-4b16-91a1-67936a5cf3bf}" enabled="0" method="" siteId="{72c2d0db-a1e3-4b16-91a1-67936a5cf3bf}" removed="1"/>

</xml_diff>

<commit_message>
DOSINZAGE2-671: Added modality to dataset
</commit_message>
<xml_diff>
--- a/dataset/Dataset_MedMij_Beeldbeschikbaarheid_1.0.0-beta.1.xlsx
+++ b/dataset/Dataset_MedMij_Beeldbeschikbaarheid_1.0.0-beta.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luudslagter/Documents/git/MedMij-R4-ImageAvailability/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74104CF2-C1C7-2D4D-B889-A22058A398B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52699650-1832-EE42-A460-438C8D32D7D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29540" yWindow="660" windowWidth="34160" windowHeight="27980" activeTab="1" xr2:uid="{B1E2DBBA-4EE0-4C1E-8D8A-42B6775C8263}"/>
+    <workbookView xWindow="160" yWindow="660" windowWidth="38080" windowHeight="19220" activeTab="1" xr2:uid="{B1E2DBBA-4EE0-4C1E-8D8A-42B6775C8263}"/>
   </bookViews>
   <sheets>
     <sheet name="Beeld en verslag tijdlijn raadp" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name=" Beeld &amp;Verslag beschikbaar" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Beeld en verslag tijdlijn besch'!$A$1:$N$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Beeld en verslag tijdlijn besch'!$A$1:$N$52</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="258">
   <si>
     <t>Naam</t>
   </si>
@@ -608,9 +608,6 @@
     <t>bbs-dataelement-67</t>
   </si>
   <si>
-    <t>Beeldvormend onderzoek voor beeld en verslag: subset Beeldinformatie</t>
-  </si>
-  <si>
     <t>2.2.1.BeeldinformatieIdentificatienummer</t>
   </si>
   <si>
@@ -659,9 +656,6 @@
     <t>bbs-dataelement-100</t>
   </si>
   <si>
-    <t xml:space="preserve">Wereldwijd uniek ID voor het verslag </t>
-  </si>
-  <si>
     <t>Verslaginformatie</t>
   </si>
   <si>
@@ -708,9 +702,6 @@
   </si>
   <si>
     <t>2.1.1. BeeldinformatieIdentificatienummer</t>
-  </si>
-  <si>
-    <t>2.1.2.DatumTijd</t>
   </si>
   <si>
     <t>2.1.3. BeeldTitel</t>
@@ -777,13 +768,64 @@
   </si>
   <si>
     <t xml:space="preserve">Lokaal uniek ID (in het RIS) die is toegekend aan het onderzoek. </t>
+  </si>
+  <si>
+    <t>Dit zijn de beelden zelf. In het geval van DICOM zijn deze beelden gestructureerd in Series.</t>
+  </si>
+  <si>
+    <t>Dit is het verslag zelf.</t>
+  </si>
+  <si>
+    <t>2.1.2.BeeldDatumTijd</t>
+  </si>
+  <si>
+    <t>2.2.4. Modaliteit</t>
+  </si>
+  <si>
+    <t>bbs-medmij-dataelement-5</t>
+  </si>
+  <si>
+    <t>1..*</t>
+  </si>
+  <si>
+    <t>De titel van het verslag.</t>
+  </si>
+  <si>
+    <t>Wereldwijd uniek ID voor het verslag  (in DICOM kan hiervoor study/series UID gebruikt worden).</t>
+  </si>
+  <si>
+    <t>Wereldwijd uniek ID die de set beelden omschrijft (in DICOM kan hiervoor study/series UID gebruikt worden).</t>
+  </si>
+  <si>
+    <t>Beeldvormend onderzoek voor beeld en verslag: subset Beeldinformatie.</t>
+  </si>
+  <si>
+    <t>Beeldvormend onderzoek voor beeld en verslag: subset Verslag.</t>
+  </si>
+  <si>
+    <t>Anatomische locatie die de focus is van de verrichting.</t>
+  </si>
+  <si>
+    <t>Lateraliteit verbijzondert de anatomische locatie door, indien van toepassing, de zijdigheid vast te leggen, bijvoorbeeld links.</t>
+  </si>
+  <si>
+    <t>Wereldwijd uniek ID voor het verslag (in DICOM kan hiervoor study/series UID gebruikt worden).</t>
+  </si>
+  <si>
+    <t>De titel van het beeld.</t>
+  </si>
+  <si>
+    <t>Het medische beeldvormingsapparaat, zoals een CT-scanner of een MRI-machine, dat wordt gebruikt om de beelden te verkrijgen.</t>
+  </si>
+  <si>
+    <t>Modalities</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1179,7 +1221,7 @@
     <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1293,13 +1335,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="25" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="25" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="25" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="25" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1662,7 +1708,7 @@
       <selection activeCell="G1" activeCellId="1" sqref="F1:F1048576 G1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.5" customWidth="1"/>
     <col min="2" max="5" width="11" customWidth="1"/>
@@ -1670,7 +1716,7 @@
     <col min="7" max="241" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1">
+    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1708,61 +1754,56 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="2" customFormat="1" ht="2" customHeight="1">
-      <c r="A2" s="53" t="s">
+    <row r="2" spans="1:12" s="2" customFormat="1" ht="2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="53" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="53" t="s">
+      <c r="C2" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="57" t="s">
+      <c r="E2" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="53" t="s">
+      <c r="F2" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="53" t="s">
+      <c r="G2" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="53" t="s">
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="53" t="s">
+      <c r="K2" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="57" t="s">
+      <c r="L2" s="56" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="2" customFormat="1">
-      <c r="A3" s="54"/>
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="56"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="58"/>
+    <row r="3" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="55"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="G2:G3"/>
@@ -1770,6 +1811,11 @@
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="J2:J3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L2" r:id="rId1" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.0.1.7&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{3CDAD70A-3BBE-4CDA-810F-FA2B5C6B897A}"/>
@@ -1781,13 +1827,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B30DEB3F-E859-4BC8-9057-6D7475D627C0}">
-  <dimension ref="A1:O53"/>
+  <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.5" style="51" customWidth="1"/>
     <col min="2" max="2" width="21.83203125" style="52" customWidth="1"/>
@@ -1798,7 +1844,7 @@
     <col min="242" max="16384" width="8.83203125" style="52"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="10" customFormat="1">
+    <row r="1" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
@@ -1836,7 +1882,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="37" customFormat="1">
+    <row r="2" spans="1:15" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="34" t="s">
         <v>22</v>
       </c>
@@ -1860,7 +1906,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="10" customFormat="1">
+    <row r="3" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="38" t="s">
         <v>27</v>
       </c>
@@ -1887,7 +1933,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="10" customFormat="1">
+    <row r="4" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="39" t="s">
         <v>31</v>
       </c>
@@ -1919,7 +1965,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="10" customFormat="1">
+    <row r="5" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="40" t="s">
         <v>38</v>
       </c>
@@ -1949,7 +1995,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="10" customFormat="1">
+    <row r="6" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="39" t="s">
         <v>42</v>
       </c>
@@ -1981,7 +2027,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="10" customFormat="1">
+    <row r="7" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="39" t="s">
         <v>47</v>
       </c>
@@ -2013,7 +2059,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="10" customFormat="1" ht="17.25" customHeight="1">
+    <row r="8" spans="1:15" s="10" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="41" t="s">
         <v>51</v>
       </c>
@@ -2045,7 +2091,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="10" customFormat="1" ht="18.75" customHeight="1">
+    <row r="9" spans="1:15" s="10" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="42" t="s">
         <v>53</v>
       </c>
@@ -2077,7 +2123,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="10" customFormat="1">
+    <row r="10" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="42" t="s">
         <v>59</v>
       </c>
@@ -2111,7 +2157,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="10" customFormat="1">
+    <row r="11" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="43" t="s">
         <v>65</v>
       </c>
@@ -2137,7 +2183,7 @@
       <c r="K11" s="37"/>
       <c r="L11" s="36"/>
     </row>
-    <row r="12" spans="1:15" s="10" customFormat="1">
+    <row r="12" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="44" t="s">
         <v>69</v>
       </c>
@@ -2167,7 +2213,7 @@
       </c>
       <c r="L12" s="36"/>
     </row>
-    <row r="13" spans="1:15" s="10" customFormat="1">
+    <row r="13" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="39" t="s">
         <v>74</v>
       </c>
@@ -2197,7 +2243,7 @@
       </c>
       <c r="L13" s="36"/>
     </row>
-    <row r="14" spans="1:15" s="10" customFormat="1">
+    <row r="14" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="39" t="s">
         <v>78</v>
       </c>
@@ -2229,7 +2275,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="10" customFormat="1" ht="105">
+    <row r="15" spans="1:15" s="10" customFormat="1" ht="105" x14ac:dyDescent="0.2">
       <c r="A15" s="39" t="s">
         <v>82</v>
       </c>
@@ -2246,7 +2292,7 @@
         <v>61</v>
       </c>
       <c r="F15" s="31" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="G15" s="37"/>
       <c r="H15" s="37"/>
@@ -2264,7 +2310,7 @@
       <c r="N15" s="45"/>
       <c r="O15" s="45"/>
     </row>
-    <row r="16" spans="1:15" s="10" customFormat="1" ht="16" customHeight="1">
+    <row r="16" spans="1:15" s="10" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="40" t="s">
         <v>85</v>
       </c>
@@ -2278,7 +2324,9 @@
         <v>33</v>
       </c>
       <c r="E16" s="36"/>
-      <c r="F16" s="45"/>
+      <c r="F16" s="47" t="s">
+        <v>252</v>
+      </c>
       <c r="G16" s="37"/>
       <c r="H16" s="36" t="s">
         <v>87</v>
@@ -2292,7 +2340,7 @@
       </c>
       <c r="L16" s="36"/>
     </row>
-    <row r="17" spans="1:12" s="37" customFormat="1">
+    <row r="17" spans="1:12" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="46" t="s">
         <v>88</v>
       </c>
@@ -2325,7 +2373,7 @@
       </c>
       <c r="L17" s="36"/>
     </row>
-    <row r="18" spans="1:12" s="10" customFormat="1">
+    <row r="18" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
         <v>94</v>
       </c>
@@ -2341,8 +2389,11 @@
       <c r="E18" s="12" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" s="10" customFormat="1" ht="16" customHeight="1">
+      <c r="F18" s="11" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" s="10" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
         <v>97</v>
       </c>
@@ -2372,7 +2423,7 @@
       </c>
       <c r="L19" s="36"/>
     </row>
-    <row r="20" spans="1:12" s="10" customFormat="1">
+    <row r="20" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="48" t="s">
         <v>101</v>
       </c>
@@ -2402,7 +2453,7 @@
       </c>
       <c r="L20" s="36"/>
     </row>
-    <row r="21" spans="1:12" s="10" customFormat="1" ht="15" customHeight="1">
+    <row r="21" spans="1:12" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="39" t="s">
         <v>105</v>
       </c>
@@ -2434,7 +2485,7 @@
       </c>
       <c r="L21" s="36"/>
     </row>
-    <row r="22" spans="1:12" s="10" customFormat="1" ht="18" customHeight="1">
+    <row r="22" spans="1:12" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="39" t="s">
         <v>110</v>
       </c>
@@ -2466,7 +2517,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="1:12" s="10" customFormat="1">
+    <row r="23" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="39" t="s">
         <v>114</v>
       </c>
@@ -2498,7 +2549,7 @@
       </c>
       <c r="L23" s="36"/>
     </row>
-    <row r="24" spans="1:12" s="10" customFormat="1">
+    <row r="24" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
         <v>118</v>
       </c>
@@ -2530,7 +2581,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="25" spans="1:12" s="10" customFormat="1">
+    <row r="25" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="40" t="s">
         <v>123</v>
       </c>
@@ -2558,7 +2609,7 @@
       </c>
       <c r="L25" s="36"/>
     </row>
-    <row r="26" spans="1:12" s="10" customFormat="1">
+    <row r="26" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
         <v>126</v>
       </c>
@@ -2588,7 +2639,7 @@
       </c>
       <c r="L26" s="36"/>
     </row>
-    <row r="27" spans="1:12" s="10" customFormat="1">
+    <row r="27" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="39" t="s">
         <v>131</v>
       </c>
@@ -2620,7 +2671,7 @@
       </c>
       <c r="L27" s="36"/>
     </row>
-    <row r="28" spans="1:12" s="10" customFormat="1" ht="16.5" customHeight="1">
+    <row r="28" spans="1:12" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="40" t="s">
         <v>136</v>
       </c>
@@ -2650,7 +2701,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="29" spans="1:12" s="10" customFormat="1">
+    <row r="29" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="39" t="s">
         <v>140</v>
       </c>
@@ -2682,7 +2733,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="30" spans="1:12" s="10" customFormat="1">
+    <row r="30" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="40" t="s">
         <v>144</v>
       </c>
@@ -2712,7 +2763,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="31" spans="1:12" s="10" customFormat="1">
+    <row r="31" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="39" t="s">
         <v>147</v>
       </c>
@@ -2744,7 +2795,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="32" spans="1:12" s="10" customFormat="1">
+    <row r="32" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="39" t="s">
         <v>151</v>
       </c>
@@ -2776,7 +2827,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="33" spans="1:12" s="10" customFormat="1">
+    <row r="33" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="39" t="s">
         <v>155</v>
       </c>
@@ -2810,7 +2861,7 @@
       </c>
       <c r="L33" s="36"/>
     </row>
-    <row r="34" spans="1:12" s="37" customFormat="1">
+    <row r="34" spans="1:12" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="40" t="s">
         <v>160</v>
       </c>
@@ -2835,7 +2886,7 @@
       </c>
       <c r="L34" s="36"/>
     </row>
-    <row r="35" spans="1:12" s="10" customFormat="1">
+    <row r="35" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
         <v>163</v>
       </c>
@@ -2863,7 +2914,7 @@
       </c>
       <c r="L35" s="12"/>
     </row>
-    <row r="36" spans="1:12" s="10" customFormat="1">
+    <row r="36" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="39" t="s">
         <v>166</v>
       </c>
@@ -2895,7 +2946,7 @@
       </c>
       <c r="L36" s="36"/>
     </row>
-    <row r="37" spans="1:12" s="10" customFormat="1" ht="18" customHeight="1">
+    <row r="37" spans="1:12" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="40" t="s">
         <v>168</v>
       </c>
@@ -2925,7 +2976,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="38" spans="1:12" s="10" customFormat="1">
+    <row r="38" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="39" t="s">
         <v>170</v>
       </c>
@@ -2957,7 +3008,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="39" spans="1:12" s="10" customFormat="1">
+    <row r="39" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="40" t="s">
         <v>172</v>
       </c>
@@ -2987,7 +3038,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="40" spans="1:12" s="10" customFormat="1">
+    <row r="40" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="39" t="s">
         <v>174</v>
       </c>
@@ -3019,7 +3070,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="41" spans="1:12" s="10" customFormat="1">
+    <row r="41" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="39" t="s">
         <v>176</v>
       </c>
@@ -3051,7 +3102,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="42" spans="1:12" s="10" customFormat="1">
+    <row r="42" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="39" t="s">
         <v>178</v>
       </c>
@@ -3085,7 +3136,7 @@
       </c>
       <c r="L42" s="36"/>
     </row>
-    <row r="43" spans="1:12" s="10" customFormat="1">
+    <row r="43" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="39" t="s">
         <v>180</v>
       </c>
@@ -3119,7 +3170,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="44" spans="1:12" s="10" customFormat="1">
+    <row r="44" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="49" t="s">
         <v>186</v>
       </c>
@@ -3134,7 +3185,7 @@
       </c>
       <c r="E44" s="36"/>
       <c r="F44" s="35" t="s">
-        <v>188</v>
+        <v>250</v>
       </c>
       <c r="G44" s="37"/>
       <c r="H44" s="37"/>
@@ -3147,12 +3198,12 @@
       </c>
       <c r="L44" s="36"/>
     </row>
-    <row r="45" spans="1:12" s="10" customFormat="1">
+    <row r="45" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="39" t="s">
+        <v>188</v>
+      </c>
+      <c r="B45" s="35" t="s">
         <v>189</v>
-      </c>
-      <c r="B45" s="35" t="s">
-        <v>190</v>
       </c>
       <c r="C45" s="35" t="s">
         <v>14</v>
@@ -3164,7 +3215,7 @@
         <v>16</v>
       </c>
       <c r="F45" s="35" t="s">
-        <v>191</v>
+        <v>249</v>
       </c>
       <c r="G45" s="37"/>
       <c r="H45" s="37"/>
@@ -3173,16 +3224,16 @@
         <v>19</v>
       </c>
       <c r="K45" s="35" t="s">
+        <v>191</v>
+      </c>
+      <c r="L45" s="36"/>
+    </row>
+    <row r="46" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="39" t="s">
         <v>192</v>
       </c>
-      <c r="L45" s="36"/>
-    </row>
-    <row r="46" spans="1:12" s="10" customFormat="1">
-      <c r="A46" s="39" t="s">
+      <c r="B46" s="35" t="s">
         <v>193</v>
-      </c>
-      <c r="B46" s="35" t="s">
-        <v>194</v>
       </c>
       <c r="C46" s="35" t="s">
         <v>14</v>
@@ -3194,7 +3245,7 @@
         <v>56</v>
       </c>
       <c r="F46" s="35" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G46" s="37"/>
       <c r="H46" s="37"/>
@@ -3203,102 +3254,104 @@
         <v>19</v>
       </c>
       <c r="K46" s="35" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="L46" s="36"/>
     </row>
-    <row r="47" spans="1:12" s="10" customFormat="1">
+    <row r="47" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="B47" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="B47" s="11" t="s">
+      <c r="C47" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D47" s="11" t="s">
         <v>197</v>
-      </c>
-      <c r="C47" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D47" s="11" t="s">
-        <v>198</v>
       </c>
       <c r="E47" s="12" t="s">
         <v>34</v>
       </c>
       <c r="F47" s="11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I47" s="12"/>
       <c r="J47" s="11" t="s">
         <v>19</v>
       </c>
       <c r="K47" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="L47" s="12"/>
     </row>
-    <row r="48" spans="1:12" s="10" customFormat="1">
-      <c r="A48" s="49" t="s">
-        <v>201</v>
+    <row r="48" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="61" t="s">
+        <v>244</v>
       </c>
       <c r="B48" s="35" t="s">
-        <v>202</v>
+        <v>245</v>
       </c>
       <c r="C48" s="35" t="s">
         <v>14</v>
       </c>
       <c r="D48" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="E48" s="36"/>
+        <v>246</v>
+      </c>
+      <c r="E48" s="36" t="s">
+        <v>61</v>
+      </c>
       <c r="F48" s="35" t="s">
-        <v>232</v>
+        <v>256</v>
       </c>
       <c r="G48" s="37"/>
       <c r="H48" s="37"/>
-      <c r="I48" s="37"/>
+      <c r="I48" s="36" t="s">
+        <v>257</v>
+      </c>
       <c r="J48" s="35" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="K48" s="35" t="s">
-        <v>73</v>
+        <v>191</v>
       </c>
       <c r="L48" s="36"/>
     </row>
-    <row r="49" spans="1:12" s="10" customFormat="1">
-      <c r="A49" s="39" t="s">
-        <v>203</v>
+    <row r="49" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="49" t="s">
+        <v>200</v>
       </c>
       <c r="B49" s="35" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C49" s="35" t="s">
         <v>14</v>
       </c>
       <c r="D49" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="E49" s="36" t="s">
-        <v>16</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="E49" s="36"/>
       <c r="F49" s="35" t="s">
-        <v>205</v>
+        <v>251</v>
       </c>
       <c r="G49" s="37"/>
       <c r="H49" s="37"/>
       <c r="I49" s="37"/>
       <c r="J49" s="35" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="K49" s="35" t="s">
-        <v>206</v>
+        <v>73</v>
       </c>
       <c r="L49" s="36"/>
     </row>
-    <row r="50" spans="1:12" s="10" customFormat="1">
+    <row r="50" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="39" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B50" s="35" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C50" s="35" t="s">
         <v>14</v>
@@ -3307,10 +3360,10 @@
         <v>15</v>
       </c>
       <c r="E50" s="36" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="F50" s="35" t="s">
-        <v>209</v>
+        <v>248</v>
       </c>
       <c r="G50" s="37"/>
       <c r="H50" s="37"/>
@@ -3319,74 +3372,74 @@
         <v>19</v>
       </c>
       <c r="K50" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="L50" s="36"/>
+    </row>
+    <row r="51" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="39" t="s">
+        <v>205</v>
+      </c>
+      <c r="B51" s="35" t="s">
         <v>206</v>
       </c>
-      <c r="L50" s="36"/>
-    </row>
-    <row r="51" spans="1:12" s="10" customFormat="1">
-      <c r="A51" s="15" t="s">
-        <v>210</v>
-      </c>
-      <c r="B51" s="11" t="s">
-        <v>211</v>
-      </c>
-      <c r="C51" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D51" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="E51" s="12" t="s">
+      <c r="C51" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D51" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="E51" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="F51" s="35" t="s">
+        <v>207</v>
+      </c>
+      <c r="G51" s="37"/>
+      <c r="H51" s="37"/>
+      <c r="I51" s="37"/>
+      <c r="J51" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="K51" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="L51" s="36"/>
+    </row>
+    <row r="52" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="B52" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D52" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="E52" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="F51" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="I51" s="12"/>
-      <c r="J51" s="11" t="s">
+      <c r="F52" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="I52" s="12"/>
+      <c r="J52" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="K51" s="11" t="s">
-        <v>206</v>
-      </c>
-      <c r="L51" s="12"/>
-    </row>
-    <row r="52" spans="1:12" s="10" customFormat="1">
-      <c r="A52" s="59" t="s">
-        <v>240</v>
-      </c>
-      <c r="B52" s="35" t="s">
-        <v>238</v>
-      </c>
-      <c r="C52" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="D52" s="35" t="s">
-        <v>96</v>
-      </c>
-      <c r="E52" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="F52" s="35" t="s">
-        <v>243</v>
-      </c>
-      <c r="G52" s="37"/>
-      <c r="H52" s="37"/>
-      <c r="I52" s="36"/>
-      <c r="J52" s="35" t="s">
-        <v>19</v>
-      </c>
       <c r="K52" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="L52" s="36"/>
-    </row>
-    <row r="53" spans="1:12" s="10" customFormat="1">
-      <c r="A53" s="59" t="s">
-        <v>241</v>
+        <v>204</v>
+      </c>
+      <c r="L52" s="12"/>
+    </row>
+    <row r="53" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="53" t="s">
+        <v>237</v>
       </c>
       <c r="B53" s="35" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C53" s="35" t="s">
         <v>14</v>
@@ -3398,7 +3451,7 @@
         <v>16</v>
       </c>
       <c r="F53" s="35" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G53" s="37"/>
       <c r="H53" s="37"/>
@@ -3411,8 +3464,38 @@
       </c>
       <c r="L53" s="36"/>
     </row>
+    <row r="54" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="53" t="s">
+        <v>238</v>
+      </c>
+      <c r="B54" s="35" t="s">
+        <v>236</v>
+      </c>
+      <c r="C54" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D54" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="E54" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="F54" s="35" t="s">
+        <v>239</v>
+      </c>
+      <c r="G54" s="37"/>
+      <c r="H54" s="37"/>
+      <c r="I54" s="36"/>
+      <c r="J54" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="K54" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="L54" s="36"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:N51" xr:uid="{B30DEB3F-E859-4BC8-9057-6D7475D627C0}"/>
+  <autoFilter ref="A1:N52" xr:uid="{B30DEB3F-E859-4BC8-9057-6D7475D627C0}"/>
   <phoneticPr fontId="16" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{21527874-0ADF-4209-82A0-BEEB3929A2FA}"/>
@@ -3482,12 +3565,12 @@
     <hyperlink ref="L45" r:id="rId65" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{315742DA-B29B-4B38-8898-713230484F64}"/>
     <hyperlink ref="E46" r:id="rId66" location="Datum/tijd" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Datum/tijd" xr:uid="{1DD7FB21-ADBA-43A1-8D64-769C58250348}"/>
     <hyperlink ref="L46" r:id="rId67" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{81FECE2A-75A0-4F3C-B166-B8CF5C058228}"/>
-    <hyperlink ref="E48" r:id="rId68" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{49D5FF9B-FE40-43A6-A865-3F174F2030FA}"/>
-    <hyperlink ref="L48" r:id="rId69" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{4FAB496D-24B1-47A2-A9A0-9552D567398B}"/>
-    <hyperlink ref="E49" r:id="rId70" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{7B8E1B66-0D74-498D-8D88-C6351C4F7FB1}"/>
-    <hyperlink ref="L49" r:id="rId71" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{E05351A4-8368-4A4B-B12F-961BE504A1A5}"/>
-    <hyperlink ref="E50" r:id="rId72" location="Datum/tijd" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Datum/tijd" xr:uid="{B9A776CF-FC80-4D4E-9655-984F31074E85}"/>
-    <hyperlink ref="L50" r:id="rId73" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{A19CC1FA-FBE7-46A2-A89E-FC0E605879FD}"/>
+    <hyperlink ref="E49" r:id="rId68" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset" xr:uid="{49D5FF9B-FE40-43A6-A865-3F174F2030FA}"/>
+    <hyperlink ref="L49" r:id="rId69" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{4FAB496D-24B1-47A2-A9A0-9552D567398B}"/>
+    <hyperlink ref="E50" r:id="rId70" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{7B8E1B66-0D74-498D-8D88-C6351C4F7FB1}"/>
+    <hyperlink ref="L50" r:id="rId71" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{E05351A4-8368-4A4B-B12F-961BE504A1A5}"/>
+    <hyperlink ref="E51" r:id="rId72" location="Datum/tijd" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Datum/tijd" xr:uid="{B9A776CF-FC80-4D4E-9655-984F31074E85}"/>
+    <hyperlink ref="L51" r:id="rId73" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=&amp;conceptEffectiveDate=&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{A19CC1FA-FBE7-46A2-A89E-FC0E605879FD}"/>
     <hyperlink ref="L24" r:id="rId74" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.17.2.4&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{6F907670-FA22-4633-9957-BF1722D97459}"/>
     <hyperlink ref="I24" r:id="rId75" display="http://decor.nictiz.nl/decor/services/RetrieveValueSet?prefix=bbs-&amp;id=2.16.840.1.113883.2.4.3.11.60.40.2.17.2.3&amp;effectiveDate=2020-09-01T00:00:00&amp;version=2024-02-08T09:28:09&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{A620A0BE-0D93-418C-8E02-69F661FAE5FD}"/>
     <hyperlink ref="E24" r:id="rId76" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{6429EA44-A0BE-46EC-BF67-7430BB9AAE0F}"/>
@@ -3528,8 +3611,10 @@
     <hyperlink ref="H17" r:id="rId111" display="http://decor.nictiz.nl/decor/services/RedirectTerminology?codeSystem=2.16.840.1.113883.6.96&amp;conceptId=363698007&amp;language=nl-NL&amp;prefix=bbs-&amp;version=2024-02-08T09:28:09" xr:uid="{58172FD2-70FC-4673-BF70-D6AE18467415}"/>
     <hyperlink ref="E17" r:id="rId112" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{3D0023D3-652A-4840-9808-3B2E5DA099D0}"/>
     <hyperlink ref="E18" r:id="rId113" location="/bbs-/terminology/valueset/2.16.840.1.113883.2.4.3.11.60.40.2.20.7.2/2020-09-01T00:00:00" xr:uid="{4B3833E8-D6ED-4EC3-8D1E-0F1FF55B206E}"/>
-    <hyperlink ref="E52" r:id="rId114" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{06898B6A-A0ED-0244-9A16-72B56DEBED42}"/>
-    <hyperlink ref="E53" r:id="rId115" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{EABED256-857D-2642-BE3E-5AD20C03336E}"/>
+    <hyperlink ref="E53" r:id="rId114" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{06898B6A-A0ED-0244-9A16-72B56DEBED42}"/>
+    <hyperlink ref="E54" r:id="rId115" location="Identificatie" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Identificatie" xr:uid="{EABED256-857D-2642-BE3E-5AD20C03336E}"/>
+    <hyperlink ref="E48" r:id="rId116" location="Code" display="https://art-decor.org/mediawiki/index.php?title=DECOR-dataset - Code" xr:uid="{0BB16F56-88D4-5644-B710-8B7860CB1712}"/>
+    <hyperlink ref="I48" r:id="rId117" xr:uid="{E48A8B75-06B7-5444-866E-89BA6FC9A9FC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3543,13 +3628,13 @@
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.5" customWidth="1"/>
     <col min="2" max="241" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1">
+    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3572,7 +3657,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
@@ -3587,7 +3672,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="2" customFormat="1" ht="68" customHeight="1">
+    <row r="2" spans="1:12" s="2" customFormat="1" ht="68" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
@@ -3620,12 +3705,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="2" customFormat="1">
+    <row r="3" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>14</v>
@@ -3637,23 +3722,23 @@
         <v>16</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H3" s="29"/>
       <c r="J3" s="4" t="s">
         <v>19</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" s="2" customFormat="1">
+    <row r="4" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>14</v>
@@ -3665,14 +3750,14 @@
         <v>16</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H4" s="28"/>
       <c r="J4" s="4" t="s">
         <v>19</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="L4" s="3"/>
     </row>
@@ -3693,11 +3778,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4A01627-17D2-4A39-A8A2-B1EFC11356BF}">
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33.33203125" style="18" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
@@ -3706,7 +3791,7 @@
     <col min="7" max="241" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1">
+    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -3744,9 +3829,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="2" customFormat="1">
+    <row r="2" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>23</v>
@@ -3768,7 +3853,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="2" customFormat="1">
+    <row r="3" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
         <v>27</v>
       </c>
@@ -3795,7 +3880,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="2" customFormat="1">
+    <row r="4" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>31</v>
       </c>
@@ -3824,7 +3909,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="2" customFormat="1">
+    <row r="5" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>38</v>
       </c>
@@ -3851,7 +3936,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="2" customFormat="1">
+    <row r="6" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>42</v>
       </c>
@@ -3868,7 +3953,7 @@
         <v>34</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>19</v>
@@ -3880,7 +3965,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="2" customFormat="1">
+    <row r="7" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>47</v>
       </c>
@@ -3909,7 +3994,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="8" spans="1:14" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="24" t="s">
         <v>51</v>
       </c>
@@ -3941,7 +4026,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="2" customFormat="1" ht="18" customHeight="1">
+    <row r="9" spans="1:14" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="24" t="s">
         <v>53</v>
       </c>
@@ -3958,7 +4043,7 @@
         <v>56</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>19</v>
@@ -3970,7 +4055,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:14" s="2" customFormat="1">
+    <row r="10" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="24" t="s">
         <v>59</v>
       </c>
@@ -3987,7 +4072,7 @@
         <v>61</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>63</v>
@@ -4002,7 +4087,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="2" customFormat="1">
+    <row r="11" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="27" t="s">
         <v>65</v>
       </c>
@@ -4028,22 +4113,22 @@
       <c r="K11" s="21"/>
       <c r="L11" s="22"/>
     </row>
-    <row r="12" spans="1:14" s="2" customFormat="1">
+    <row r="12" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B12" s="20" t="s">
         <v>187</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D12" s="20" t="s">
         <v>33</v>
       </c>
       <c r="E12" s="22"/>
       <c r="F12" s="20" t="s">
-        <v>188</v>
+        <v>250</v>
       </c>
       <c r="G12" s="21"/>
       <c r="H12" s="21"/>
@@ -4056,12 +4141,12 @@
       </c>
       <c r="L12" s="22"/>
     </row>
-    <row r="13" spans="1:14" s="2" customFormat="1">
+    <row r="13" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="23" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C13" s="20" t="s">
         <v>14</v>
@@ -4073,7 +4158,7 @@
         <v>16</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>191</v>
+        <v>249</v>
       </c>
       <c r="G13" s="21"/>
       <c r="H13" s="21"/>
@@ -4082,16 +4167,16 @@
         <v>19</v>
       </c>
       <c r="K13" s="20" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="L13" s="22"/>
     </row>
-    <row r="14" spans="1:14" s="2" customFormat="1">
+    <row r="14" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
-        <v>222</v>
+        <v>243</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C14" s="20" t="s">
         <v>14</v>
@@ -4103,7 +4188,7 @@
         <v>56</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
@@ -4112,54 +4197,57 @@
         <v>19</v>
       </c>
       <c r="K14" s="20" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="L14" s="22"/>
     </row>
-    <row r="15" spans="1:14" s="2" customFormat="1">
+    <row r="15" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>197</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>198</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>34</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>200</v>
+        <v>255</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="K15" s="3"/>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
       <c r="N15" s="3"/>
     </row>
-    <row r="16" spans="1:14" s="2" customFormat="1">
+    <row r="16" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="19" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E16" s="6"/>
+      <c r="F16" s="60" t="s">
+        <v>241</v>
+      </c>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
@@ -4167,22 +4255,22 @@
       <c r="K16" s="5"/>
       <c r="L16" s="6"/>
     </row>
-    <row r="17" spans="1:14" s="2" customFormat="1">
+    <row r="17" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B17" s="20" t="s">
         <v>187</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D17" s="20" t="s">
         <v>33</v>
       </c>
       <c r="E17" s="22"/>
       <c r="F17" s="20" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="G17" s="21"/>
       <c r="H17" s="21"/>
@@ -4195,12 +4283,12 @@
       </c>
       <c r="L17" s="22"/>
     </row>
-    <row r="18" spans="1:14" s="2" customFormat="1">
+    <row r="18" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C18" s="20" t="s">
         <v>14</v>
@@ -4212,7 +4300,7 @@
         <v>16</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>205</v>
+        <v>254</v>
       </c>
       <c r="G18" s="21"/>
       <c r="H18" s="21"/>
@@ -4221,16 +4309,16 @@
         <v>19</v>
       </c>
       <c r="K18" s="20" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="L18" s="22"/>
     </row>
-    <row r="19" spans="1:14" s="2" customFormat="1">
+    <row r="19" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="23" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C19" s="20" t="s">
         <v>14</v>
@@ -4242,7 +4330,7 @@
         <v>56</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G19" s="21"/>
       <c r="H19" s="21"/>
@@ -4251,46 +4339,46 @@
         <v>19</v>
       </c>
       <c r="K19" s="20" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="L19" s="22"/>
     </row>
-    <row r="20" spans="1:14" s="2" customFormat="1">
+    <row r="20" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>34</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>212</v>
+        <v>247</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="K20" s="3"/>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
       <c r="N20" s="3"/>
     </row>
-    <row r="21" spans="1:14" s="4" customFormat="1" ht="14">
+    <row r="21" spans="1:14" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>14</v>
@@ -4299,15 +4387,18 @@
         <v>15</v>
       </c>
       <c r="E21" s="9"/>
-    </row>
-    <row r="23" spans="1:14">
+      <c r="F21" s="60" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="18" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="30" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -4368,15 +4459,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100597771DCE5E0DD409E6796B5544574D3" ma:contentTypeVersion="14" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="1f155c61874143f60c84865cea76726f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7be6589a-2b09-4451-a4d9-5c4f513f6c62" xmlns:ns3="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7515b2bcca035c7557d524d6ba7a724c" ns2:_="" ns3:_="">
     <xsd:import namespace="7be6589a-2b09-4451-a4d9-5c4f513f6c62"/>
@@ -4605,6 +4687,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A9F8A2F-C3FF-4FEC-AF19-26E26DE76F65}">
   <ds:schemaRefs>
@@ -4617,14 +4708,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD20EF80-7752-41E2-9F6E-5CDF83210C62}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{815FF2A9-0500-4E41-8F16-110FB0128C02}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4643,6 +4726,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD20EF80-7752-41E2-9F6E-5CDF83210C62}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{72c2d0db-a1e3-4b16-91a1-67936a5cf3bf}" enabled="0" method="" siteId="{72c2d0db-a1e3-4b16-91a1-67936a5cf3bf}" removed="1"/>

</xml_diff>